<commit_message>
updated by Shuvayan on 24-07-2023
updated by Shuvayan on 24-07-2023
</commit_message>
<xml_diff>
--- a/Offline/BusinessManagement/Teach_Tech@anodiam/IT/IT-LogBook.xlsx
+++ b/Offline/BusinessManagement/Teach_Tech@anodiam/IT/IT-LogBook.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Anodiam\Docs\Offline\BusinessManagement\Teach_Tech@anodiam\IT\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD0A7327-B81D-41F9-AAE9-E9CC685F4882}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19440" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="Shuvayan" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Date</t>
   </si>
@@ -34,12 +28,21 @@
   </si>
   <si>
     <t>Remarks</t>
+  </si>
+  <si>
+    <t>24/7/2023</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>Online meeting with Classplus</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -131,7 +134,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -166,7 +169,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -343,23 +346,26 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="28.42578125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -368,6 +374,17 @@
       </c>
       <c r="C1" t="s">
         <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Advertisement in facebook is in progress
Advertisement in facebook is in progress
</commit_message>
<xml_diff>
--- a/Offline/BusinessManagement/Teach_Tech@anodiam/IT/IT-LogBook.xlsx
+++ b/Offline/BusinessManagement/Teach_Tech@anodiam/IT/IT-LogBook.xlsx
@@ -1,13 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Anodiam\Docs\Offline\BusinessManagement\Teach_Tech@anodiam\IT\CourseMaterials\Java\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEFCB1D0-D915-449F-A63C-DB7B627F0768}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19440" windowHeight="7755"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Shuvayan" sheetId="1" r:id="rId1"/>
+    <sheet name="Shubhayan" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -19,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="15">
   <si>
     <t>Date</t>
   </si>
@@ -37,12 +43,39 @@
   </si>
   <si>
     <t>Online meeting with Classplus</t>
+  </si>
+  <si>
+    <t>27/7/2023</t>
+  </si>
+  <si>
+    <t>IT</t>
+  </si>
+  <si>
+    <t>Making slides 4,5 for Java</t>
+  </si>
+  <si>
+    <t>Writing small sample programs</t>
+  </si>
+  <si>
+    <t>13/7/2023</t>
+  </si>
+  <si>
+    <t>14/7/2023</t>
+  </si>
+  <si>
+    <t>Disrcussion regarding Collection Classes</t>
+  </si>
+  <si>
+    <t>21/7/2023</t>
+  </si>
+  <si>
+    <t>Discussion regarding Slides. Made slide 3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -72,8 +105,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -134,7 +168,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -169,7 +203,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -346,26 +380,28 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="B2" sqref="B2:B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="28.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="37.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -376,15 +412,70 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="1">
+        <v>45267</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B6" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C6" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>